<commit_message>
modified the mission planning script, creates a monthly data seprated by dev, algo and bi while each divider has a column of company name according to the budget name
</commit_message>
<xml_diff>
--- a/src/excel/evogene-jira-analist/budget-naming.xlsx
+++ b/src/excel/evogene-jira-analist/budget-naming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\utils\src\excel\evogene-jira-analist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BE2783-21F9-47F4-958B-168EFBC9FC2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D275370B-1BFD-4AC9-8139-EB8953709C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
   <si>
     <t>budget</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t>CPB</t>
+  </si>
+  <si>
+    <t>P144</t>
+  </si>
+  <si>
+    <t>P997</t>
+  </si>
+  <si>
+    <t>Upkeep</t>
+  </si>
+  <si>
+    <t>P23</t>
   </si>
 </sst>
 </file>
@@ -480,9 +492,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
@@ -519,7 +533,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -527,15 +541,15 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -543,7 +557,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -551,7 +565,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -559,7 +573,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -567,7 +581,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -575,39 +589,39 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -615,7 +629,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -623,23 +637,23 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -647,7 +661,7 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -655,7 +669,7 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -663,7 +677,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -671,7 +685,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -679,7 +693,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -687,23 +701,23 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -711,7 +725,7 @@
         <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -719,7 +733,7 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -727,7 +741,7 @@
         <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -735,7 +749,7 @@
         <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -743,7 +757,7 @@
         <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -751,23 +765,23 @@
         <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -775,7 +789,7 @@
         <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -783,7 +797,7 @@
         <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -791,7 +805,31 @@
         <v>45</v>
       </c>
       <c r="B38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
creting the yearly dataframe of the time spent, modified names in the teams, as neened
</commit_message>
<xml_diff>
--- a/src/excel/evogene-jira-analist/budget-naming.xlsx
+++ b/src/excel/evogene-jira-analist/budget-naming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\utils\src\excel\evogene-jira-analist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D275370B-1BFD-4AC9-8139-EB8953709C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0544B6-2B13-4492-A76D-3B6EF1D80854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
   <si>
     <t>budget</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>P23</t>
+  </si>
+  <si>
+    <t>Chempass</t>
+  </si>
+  <si>
+    <t>MicroBoost</t>
+  </si>
+  <si>
+    <t>P22</t>
   </si>
 </sst>
 </file>
@@ -492,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -557,7 +566,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -565,7 +574,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -573,7 +582,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -581,7 +590,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -589,7 +598,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -597,7 +606,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -605,15 +614,15 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -621,15 +630,15 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -637,7 +646,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -645,7 +654,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -653,15 +662,15 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -669,7 +678,7 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -677,7 +686,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -685,7 +694,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -693,7 +702,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -701,7 +710,7 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -709,7 +718,7 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -717,47 +726,47 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -765,7 +774,7 @@
         <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -773,7 +782,7 @@
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -781,15 +790,15 @@
         <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -797,7 +806,7 @@
         <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -805,7 +814,7 @@
         <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -813,7 +822,7 @@
         <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -821,14 +830,22 @@
         <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>48</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
styling the excel' adding total columns
</commit_message>
<xml_diff>
--- a/src/excel/evogene-jira-analist/budget-naming.xlsx
+++ b/src/excel/evogene-jira-analist/budget-naming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\utils\src\excel\evogene-jira-analist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0544B6-2B13-4492-A76D-3B6EF1D80854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5545DF99-436C-4D5A-938E-4E5A2E7342EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
   <si>
     <t>budget</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>P22</t>
+  </si>
+  <si>
+    <t>Crispril</t>
   </si>
 </sst>
 </file>
@@ -219,8 +222,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -770,16 +775,16 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>39</v>
+      <c r="A33" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="B33" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>39</v>
+      <c r="A34" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="B34" t="s">
         <v>36</v>

</xml_diff>